<commit_message>
Source data extraction from sources 1 through 9
</commit_message>
<xml_diff>
--- a/Research Corpus/Data by Source/Source_1|3D-DAG- Scaling Blockchain via DAG.xlsx
+++ b/Research Corpus/Data by Source/Source_1|3D-DAG- Scaling Blockchain via DAG.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yawu/Desktop/Repos/FT324_SLR/Research Corpus/Data by Source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BD3EC22-57AE-304C-A6BE-FBF269E6095C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E149D45D-4652-D44C-BC13-9D17C0662F83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="1000" windowWidth="27640" windowHeight="15880" xr2:uid="{754419C1-0F3F-3647-A532-9827BA1C8B7E}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="17">
   <si>
     <t>Consensus</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>DAGs</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -504,7 +507,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -545,55 +548,209 @@
       <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="1"/>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="1"/>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="1"/>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="1"/>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="1"/>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="1"/>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="1"/>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="1"/>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="1"/>
+      <c r="B10">
+        <v>98200</v>
+      </c>
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="1">
+        <f>AVERAGE(0.33,0.51)</f>
+        <v>0.42000000000000004</v>
+      </c>
+      <c r="F10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>